<commit_message>
Correção de BUGS Tirei o type bugado e esquisito
</commit_message>
<xml_diff>
--- a/Codigos/database/clientes.xlsx
+++ b/Codigos/database/clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,7 +453,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0f89ce52-f0ab-45de-96c0-c0c74cbcc982</t>
+          <t>a0250d49-275b-4792-9531-82a1aa23e91e</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -470,7 +470,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>858b4947-f2ea-4e0b-aed2-ab126d4142bb</t>
+          <t>898e3b3a-3115-45bd-bbcb-d5bcabeb41c0</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -480,58 +480,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>email.com</t>
+          <t>joaquim@example.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7b22e03c-be40-43df-932c-bd93fe5053d2</t>
+          <t>9e7b33d3-42c9-4af7-8c12-40da112137f6</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>MarceloTz</t>
+          <t>Perez</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CelindoTz@gmail.com</t>
+          <t>perez@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>c9bdb3ac-54ee-4cb8-b3dd-ab448aa47b51</t>
+          <t>74340479-d55a-41ed-b3d0-89249e2bcc5b</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Paulo</t>
+          <t>Peraldo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>paulo@email.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>4f20f150-9a1a-4678-9cd8-e06858a8c236</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>RonaldoPericles</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Pericles@ronaldo</t>
+          <t>perez2@gmail.com</t>
         </is>
       </c>
     </row>

</xml_diff>